<commit_message>
first round of tweaks
Signed-off-by: Craig Jellick <craig@acorn.io>
</commit_message>
<xml_diff>
--- a/yoy_sales.xlsx
+++ b/yoy_sales.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05EAAB08-0D76-4B27-92FC-8ACA8323A344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjellick/projects/scratch-gptscripts/scrape-regional-sales/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4852778-FF08-7649-95EE-BF038D504030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="85760" yWindow="-2080" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +53,6 @@
     <t>YoY Sales Growth (%)</t>
   </si>
   <si>
-    <t>Scranton PA</t>
-  </si>
-  <si>
     <t>SKU_001</t>
   </si>
   <si>
@@ -81,38 +83,41 @@
     <t>SKU_010</t>
   </si>
   <si>
-    <t>Stamford CT</t>
-  </si>
-  <si>
-    <t>Nashua NH</t>
-  </si>
-  <si>
-    <t>Utica NY</t>
-  </si>
-  <si>
-    <t>Albany NY</t>
-  </si>
-  <si>
-    <t>Akron OH</t>
-  </si>
-  <si>
-    <t>Camden NJ</t>
-  </si>
-  <si>
-    <t>Yonkers NY</t>
-  </si>
-  <si>
-    <t>Rochester NY</t>
-  </si>
-  <si>
-    <t>Syracuse NY</t>
+    <t>Rochester</t>
+  </si>
+  <si>
+    <t>Yonkers</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Camden</t>
+  </si>
+  <si>
+    <t>Scranton</t>
+  </si>
+  <si>
+    <t>Stamford</t>
+  </si>
+  <si>
+    <t>Nashua</t>
+  </si>
+  <si>
+    <t>Utica</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>Akron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +155,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,22 +490,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,12 +522,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>2973.91</v>
@@ -534,12 +539,12 @@
         <v>9.16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>35703.440000000002</v>
@@ -551,12 +556,12 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>9129.31</v>
@@ -565,15 +570,15 @@
         <v>9565.68</v>
       </c>
       <c r="E4">
-        <v>4.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18">
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>7513.05</v>
@@ -582,15 +587,15 @@
         <v>7888.7</v>
       </c>
       <c r="E5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>5619.56</v>
@@ -599,15 +604,15 @@
         <v>5895.54</v>
       </c>
       <c r="E6">
-        <v>4.91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>7514.67</v>
@@ -616,15 +621,15 @@
         <v>7880.4</v>
       </c>
       <c r="E7">
-        <v>4.87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>11963.2</v>
@@ -636,12 +641,12 @@
         <v>10.02</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>9135.9</v>
@@ -650,15 +655,15 @@
         <v>10049.49</v>
       </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>33304.1</v>
@@ -670,12 +675,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>8689.64</v>
@@ -686,13 +691,17 @@
       <c r="E11">
         <v>9.61</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18">
+      <c r="F11">
+        <f>SUM(E2:E11)/10</f>
+        <v>9.0359999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>4336</v>
@@ -701,15 +710,15 @@
         <v>4769.6000000000004</v>
       </c>
       <c r="E12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="18">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>36303.5</v>
@@ -721,12 +730,12 @@
         <v>5.14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>12735</v>
@@ -738,12 +747,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>3551.3</v>
@@ -755,12 +764,12 @@
         <v>5.29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>5476.39</v>
@@ -772,12 +781,12 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>9532.68</v>
@@ -789,12 +798,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>5772.64</v>
@@ -806,12 +815,12 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>7675.83</v>
@@ -820,15 +829,15 @@
         <v>8213.0400000000009</v>
       </c>
       <c r="E19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20">
         <v>27496.3</v>
@@ -837,15 +846,15 @@
         <v>30246.43</v>
       </c>
       <c r="E20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="18">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>20244</v>
@@ -854,15 +863,19 @@
         <v>22268.400000000001</v>
       </c>
       <c r="E21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F21">
+        <f>SUM(E12:E21)/10</f>
+        <v>4.4809999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>8217.9699999999993</v>
@@ -871,15 +884,15 @@
         <v>8618.8700000000008</v>
       </c>
       <c r="E22">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="18">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>11026.06</v>
@@ -888,15 +901,15 @@
         <v>12128.67</v>
       </c>
       <c r="E23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>5804.91</v>
@@ -905,15 +918,15 @@
         <v>6094.65</v>
       </c>
       <c r="E24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="18">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25">
         <v>4122.3599999999997</v>
@@ -922,15 +935,15 @@
         <v>4328.47</v>
       </c>
       <c r="E25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="18">
+        <v>5.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>16321.79</v>
@@ -939,15 +952,15 @@
         <v>18055.98</v>
       </c>
       <c r="E26">
-        <v>10.62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="18">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>5381.35</v>
@@ -959,12 +972,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28">
         <v>11336.31</v>
@@ -973,15 +986,15 @@
         <v>12469.94</v>
       </c>
       <c r="E28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="18">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>10137.1</v>
@@ -990,15 +1003,15 @@
         <v>11251.06</v>
       </c>
       <c r="E29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="18">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30">
         <v>22505.22</v>
@@ -1007,15 +1020,15 @@
         <v>24755.75</v>
       </c>
       <c r="E30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="18">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>15612.7</v>
@@ -1024,15 +1037,19 @@
         <v>17278.990000000002</v>
       </c>
       <c r="E31">
-        <v>10.66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="18">
+        <v>5.5</v>
+      </c>
+      <c r="F31">
+        <f>SUM(E22:E31)/10</f>
+        <v>5.5069999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>1581.2</v>
@@ -1041,15 +1058,15 @@
         <v>1660.26</v>
       </c>
       <c r="E32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="18">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33">
         <v>11787.79</v>
@@ -1061,12 +1078,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="18">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34">
         <v>2470.8000000000002</v>
@@ -1075,15 +1092,15 @@
         <v>2594.34</v>
       </c>
       <c r="E34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="18">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>8252.56</v>
@@ -1092,15 +1109,15 @@
         <v>8665.19</v>
       </c>
       <c r="E35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="18">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36">
         <v>6825.34</v>
@@ -1109,15 +1126,15 @@
         <v>7166.61</v>
       </c>
       <c r="E36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37">
         <v>3216</v>
@@ -1126,15 +1143,15 @@
         <v>3376.8</v>
       </c>
       <c r="E37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="18">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38">
         <v>12230.94</v>
@@ -1143,15 +1160,15 @@
         <v>12842.49</v>
       </c>
       <c r="E38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="18">
+        <v>17.34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>4802.3999999999996</v>
@@ -1160,15 +1177,15 @@
         <v>5042.5200000000004</v>
       </c>
       <c r="E39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="18">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40">
         <v>5949.52</v>
@@ -1177,15 +1194,15 @@
         <v>6246.99</v>
       </c>
       <c r="E40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="18">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41">
         <v>5380.56</v>
@@ -1194,15 +1211,19 @@
         <v>5649.59</v>
       </c>
       <c r="E41">
+        <v>11.3</v>
+      </c>
+      <c r="F41">
+        <f>SUM(E32:E41)/10</f>
+        <v>12.361000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="18">
-      <c r="A42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" t="s">
-        <v>6</v>
       </c>
       <c r="C42">
         <v>3082</v>
@@ -1214,12 +1235,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="18">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>7888.07</v>
@@ -1228,15 +1249,15 @@
         <v>8272.48</v>
       </c>
       <c r="E43">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="18">
+        <v>10.119999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>4767.6000000000004</v>
@@ -1245,15 +1266,15 @@
         <v>5005.9799999999996</v>
       </c>
       <c r="E44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="18">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>9212.16</v>
@@ -1262,15 +1283,15 @@
         <v>9672.77</v>
       </c>
       <c r="E45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="18">
+        <v>10.45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>6875.16</v>
@@ -1279,15 +1300,15 @@
         <v>7218.92</v>
       </c>
       <c r="E46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="18">
+        <v>10.88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C47">
         <v>3510.8</v>
@@ -1296,15 +1317,15 @@
         <v>3861.88</v>
       </c>
       <c r="E47">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="18">
+        <v>10.34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C48">
         <v>7710.81</v>
@@ -1313,15 +1334,15 @@
         <v>8086.35</v>
       </c>
       <c r="E48">
-        <v>4.87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="18">
+        <v>10.119999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49">
         <v>2610</v>
@@ -1330,15 +1351,15 @@
         <v>2730.45</v>
       </c>
       <c r="E49">
-        <v>4.6100000000000003</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="18">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50">
         <v>12186.92</v>
@@ -1347,15 +1368,15 @@
         <v>12795.76</v>
       </c>
       <c r="E50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="18">
+        <v>10.65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51">
         <v>6078.04</v>
@@ -1364,15 +1385,19 @@
         <v>6381.94</v>
       </c>
       <c r="E51">
+        <v>10.1</v>
+      </c>
+      <c r="F51">
+        <f>SUM(E42:E51)/10</f>
+        <v>10.434999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="18">
-      <c r="A52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6</v>
       </c>
       <c r="C52">
         <v>2519.1999999999998</v>
@@ -1381,15 +1406,15 @@
         <v>2652.16</v>
       </c>
       <c r="E52">
-        <v>5.29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="18">
+        <v>11.23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <v>8597.11</v>
@@ -1398,15 +1423,15 @@
         <v>9466.82</v>
       </c>
       <c r="E53">
-        <v>10.11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="18">
+        <v>13.45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54">
         <v>3967.2</v>
@@ -1415,15 +1440,15 @@
         <v>4165.5600000000004</v>
       </c>
       <c r="E54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="18">
+        <v>12.67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <v>11227.32</v>
@@ -1432,15 +1457,15 @@
         <v>11788.68</v>
       </c>
       <c r="E55">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="18">
+        <v>11.44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C56">
         <v>5828.94</v>
@@ -1449,15 +1474,15 @@
         <v>6119.39</v>
       </c>
       <c r="E56">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="18">
+        <v>13.78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C57">
         <v>1581.2</v>
@@ -1466,15 +1491,15 @@
         <v>1660.26</v>
       </c>
       <c r="E57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="18">
+        <v>12.55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C58">
         <v>11787.79</v>
@@ -1483,15 +1508,15 @@
         <v>12376.18</v>
       </c>
       <c r="E58">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="18">
+        <v>11.08</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59">
         <v>2470.8000000000002</v>
@@ -1500,15 +1525,15 @@
         <v>2594.34</v>
       </c>
       <c r="E59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="18">
+        <v>13.04</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C60">
         <v>8252.56</v>
@@ -1517,15 +1542,15 @@
         <v>8665.19</v>
       </c>
       <c r="E60">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="18">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C61">
         <v>6825.34</v>
@@ -1534,15 +1559,19 @@
         <v>7166.61</v>
       </c>
       <c r="E61">
+        <v>11.68</v>
+      </c>
+      <c r="F61">
+        <f>SUM(E52:E61)/10</f>
+        <v>12.367000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="18">
-      <c r="A62" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" t="s">
-        <v>6</v>
       </c>
       <c r="C62">
         <v>1929.38</v>
@@ -1551,15 +1580,15 @@
         <v>2122.3200000000002</v>
       </c>
       <c r="E62">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="18">
+        <v>17.45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63">
         <v>7533.4</v>
@@ -1568,15 +1597,15 @@
         <v>7880.07</v>
       </c>
       <c r="E63">
-        <v>4.6100000000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="18">
+        <v>18.11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C64">
         <v>3132.07</v>
@@ -1585,15 +1614,15 @@
         <v>3288.67</v>
       </c>
       <c r="E64">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="18">
+        <v>19.22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C65">
         <v>6429.17</v>
@@ -1602,15 +1631,15 @@
         <v>6750.63</v>
       </c>
       <c r="E65">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="18">
+        <v>17.010000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66">
         <v>3038.8</v>
@@ -1619,15 +1648,15 @@
         <v>3189.74</v>
       </c>
       <c r="E66">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="18">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C67">
         <v>455.55</v>
@@ -1636,15 +1665,15 @@
         <v>478.33</v>
       </c>
       <c r="E67">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="18">
+        <v>18.329999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C68">
         <v>5051.8100000000004</v>
@@ -1653,15 +1682,15 @@
         <v>5304.4</v>
       </c>
       <c r="E68">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="18">
+        <v>17.11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69">
         <v>835.22</v>
@@ -1670,15 +1699,15 @@
         <v>877.48</v>
       </c>
       <c r="E69">
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="18">
+        <v>18.440000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C70">
         <v>2398.9499999999998</v>
@@ -1687,15 +1716,15 @@
         <v>2518.9</v>
       </c>
       <c r="E70">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="18">
+        <v>19.09</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C71">
         <v>249.08</v>
@@ -1704,15 +1733,19 @@
         <v>261.52999999999997</v>
       </c>
       <c r="E71">
+        <v>17.5</v>
+      </c>
+      <c r="F71">
+        <f>SUM(E62:E71)/10</f>
+        <v>18.225000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="18">
-      <c r="A72" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6</v>
       </c>
       <c r="C72">
         <v>1339.85</v>
@@ -1721,15 +1754,15 @@
         <v>1406.84</v>
       </c>
       <c r="E72">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="18">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73">
         <v>7799.29</v>
@@ -1738,15 +1771,15 @@
         <v>8189.25</v>
       </c>
       <c r="E73">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="18">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C74">
         <v>1078.82</v>
@@ -1755,15 +1788,15 @@
         <v>1132.76</v>
       </c>
       <c r="E74">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="18">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C75">
         <v>5277.68</v>
@@ -1772,15 +1805,15 @@
         <v>5541.56</v>
       </c>
       <c r="E75">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="18">
+        <v>3.44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C76">
         <v>1295.23</v>
@@ -1789,15 +1822,15 @@
         <v>1359.99</v>
       </c>
       <c r="E76">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="18">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C77">
         <v>562.74</v>
@@ -1806,15 +1839,15 @@
         <v>590.88</v>
       </c>
       <c r="E77">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="18">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C78">
         <v>8685.57</v>
@@ -1823,15 +1856,15 @@
         <v>9119.85</v>
       </c>
       <c r="E78">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="18">
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79">
         <v>2018.45</v>
@@ -1840,15 +1873,15 @@
         <v>2119.37</v>
       </c>
       <c r="E79">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="18">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C80">
         <v>2302.9899999999998</v>
@@ -1857,15 +1890,15 @@
         <v>2418.14</v>
       </c>
       <c r="E80">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="18">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C81">
         <v>1394.86</v>
@@ -1874,15 +1907,19 @@
         <v>1464.61</v>
       </c>
       <c r="E81">
+        <v>3.55</v>
+      </c>
+      <c r="F81">
+        <f>SUM(E72:E81)/10</f>
+        <v>3.8789999999999991</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="18">
-      <c r="A82" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
       </c>
       <c r="C82">
         <v>803.91</v>
@@ -1891,15 +1928,15 @@
         <v>843.1</v>
       </c>
       <c r="E82">
-        <v>4.87</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="18">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83">
         <v>3013.36</v>
@@ -1908,15 +1945,15 @@
         <v>3159.02</v>
       </c>
       <c r="E83">
-        <v>4.83</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="18">
+        <v>13.13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C84">
         <v>1879.24</v>
@@ -1925,15 +1962,15 @@
         <v>1968.2</v>
       </c>
       <c r="E84">
-        <v>4.7300000000000004</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="18">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C85">
         <v>4989.8100000000004</v>
@@ -1942,15 +1979,15 @@
         <v>5239.3</v>
       </c>
       <c r="E85">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="18">
+        <v>13.88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C86">
         <v>4334.03</v>
@@ -1959,15 +1996,15 @@
         <v>4550.7299999999996</v>
       </c>
       <c r="E86">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="18">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C87">
         <v>2143.7600000000002</v>
@@ -1976,15 +2013,15 @@
         <v>2251.9499999999998</v>
       </c>
       <c r="E87">
-        <v>5.05</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="18">
+        <v>13.07</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C88">
         <v>7976.54</v>
@@ -1993,15 +2030,15 @@
         <v>8375.3700000000008</v>
       </c>
       <c r="E88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="18">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C89">
         <v>313.20999999999998</v>
@@ -2010,15 +2047,15 @@
         <v>328.87</v>
       </c>
       <c r="E89">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="18">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B90" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C90">
         <v>671.7</v>
@@ -2027,15 +2064,15 @@
         <v>705.29</v>
       </c>
       <c r="E90">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="18">
+        <v>12.91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C91">
         <v>4084.94</v>
@@ -2044,15 +2081,19 @@
         <v>4289.1899999999996</v>
       </c>
       <c r="E91">
+        <v>13.03</v>
+      </c>
+      <c r="F91">
+        <f>SUM(E82:E91)/10</f>
+        <v>12.902000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="18">
-      <c r="A92" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B92" t="s">
-        <v>6</v>
       </c>
       <c r="C92">
         <v>1929.38</v>
@@ -2061,15 +2102,15 @@
         <v>2122.3200000000002</v>
       </c>
       <c r="E92">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="18">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93">
         <v>7533.4</v>
@@ -2078,15 +2119,15 @@
         <v>7880.07</v>
       </c>
       <c r="E93">
-        <v>4.6100000000000003</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="18">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C94">
         <v>3132.07</v>
@@ -2095,15 +2136,15 @@
         <v>3288.67</v>
       </c>
       <c r="E94">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="18">
+        <v>8.77</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C95">
         <v>6429.17</v>
@@ -2112,15 +2153,15 @@
         <v>6750.63</v>
       </c>
       <c r="E95">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="18">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C96">
         <v>3038.8</v>
@@ -2129,15 +2170,15 @@
         <v>3189.74</v>
       </c>
       <c r="E96">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="18">
+        <v>6.77</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C97">
         <v>455.55</v>
@@ -2146,15 +2187,15 @@
         <v>478.33</v>
       </c>
       <c r="E97">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="18">
+        <v>7.01</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C98">
         <v>5051.8100000000004</v>
@@ -2163,15 +2204,15 @@
         <v>5304.4</v>
       </c>
       <c r="E98">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="18">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99">
         <v>835.22</v>
@@ -2180,15 +2221,15 @@
         <v>877.48</v>
       </c>
       <c r="E99">
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="18">
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100">
         <v>2398.9499999999998</v>
@@ -2197,15 +2238,15 @@
         <v>2518.9</v>
       </c>
       <c r="E100">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="18">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C101">
         <v>249.08</v>
@@ -2214,7 +2255,11 @@
         <v>261.52999999999997</v>
       </c>
       <c r="E101">
-        <v>5</v>
+        <v>8.15</v>
+      </c>
+      <c r="F101">
+        <f>SUM(E92:E101)/10</f>
+        <v>7.4720000000000013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>